<commit_message>
create a day cycle to test on vm and change cleanup function to only look for pdfs
</commit_message>
<xml_diff>
--- a/R&D Items Due_test.xlsx
+++ b/R&D Items Due_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZacV\PycharmProjects\R&amp;DRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE0F221-65CD-435E-A223-42071CAA85B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67627521-579F-4893-B025-DD1C96554E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R&amp;D Items Due_test" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Part Number</t>
   </si>
@@ -266,13 +266,13 @@
     <t>12D50155F7-1590C40C48</t>
   </si>
   <si>
-    <t>GIB HARVEST (4027)</t>
-  </si>
-  <si>
     <t>62C8256057-17C10DC14A</t>
   </si>
   <si>
-    <t>15ADB4B1FF-17C10DD090</t>
+    <t>YESTERDAY</t>
+  </si>
+  <si>
+    <t>GIB HARVEST (3000)</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,21 +572,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,10 +906,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +922,7 @@
     <col min="6" max="6" width="59.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
@@ -973,7 +958,7 @@
       </c>
       <c r="J1" s="23" t="str">
         <f ca="1">DEC2HEX(RANDBETWEEN(1,5*10^11),10)&amp;"-"&amp;DEC2HEX((TEXT(NOW(),"mmddyyhhmmss")),10)</f>
-        <v>5C276ABC6A-17C10DE724</v>
+        <v>0FBBDA2F35-19CD9328E5</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1025,7 +1010,7 @@
       <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="36" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1050,7 +1035,7 @@
         <v>45129</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="42"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1060,7 +1045,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" s="11">
         <v>64984246</v>
@@ -1071,16 +1056,16 @@
       <c r="D5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="38">
         <v>45147</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="31" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="22" t="s">
@@ -1098,12 +1083,12 @@
       <c r="D6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="36"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="22" t="s">
         <v>46</v>
       </c>
@@ -1120,521 +1105,462 @@
         <v>69</v>
       </c>
       <c r="E7" s="29">
-        <v>45197</v>
+        <v>45199</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="36"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="11">
-        <v>9090202100</v>
+        <v>9090202000</v>
       </c>
       <c r="C8" s="11">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="32">
-        <v>45197</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E8" s="29"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="11">
-        <v>9090202000</v>
-      </c>
-      <c r="C9" s="11">
-        <v>1200</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="28" t="s">
+      <c r="G8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="11">
-        <v>9090202100</v>
-      </c>
-      <c r="C10" s="11">
-        <v>8</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="35">
-        <v>45197</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="34"/>
-      <c r="I10" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="11">
-        <v>9090202000</v>
-      </c>
-      <c r="C11" s="11">
-        <v>1200</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="34"/>
-      <c r="I11" s="33" t="s">
-        <v>72</v>
-      </c>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="16">
+        <v>6613599332</v>
+      </c>
+      <c r="C9" s="16">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="17">
+        <v>45137</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="16">
+        <v>6613500125</v>
+      </c>
+      <c r="C10" s="16">
+        <v>6</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="16">
+        <v>6613500172</v>
+      </c>
+      <c r="C11" s="16">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="17">
+        <v>45143</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>68</v>
-      </c>
+      <c r="A12" s="41"/>
       <c r="B12" s="16">
-        <v>6613599332</v>
+        <v>93920565</v>
       </c>
       <c r="C12" s="16">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12" s="17">
-        <v>45137</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>45147</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="37"/>
       <c r="H12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="16">
-        <v>6613500125</v>
+        <v>6613200160</v>
       </c>
       <c r="C13" s="16">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="17">
-        <v>45143</v>
-      </c>
-      <c r="F13" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="19">
+        <v>45147</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="G13" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="16">
+        <v>6613599160</v>
+      </c>
+      <c r="C14" s="16">
+        <v>3</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="19">
+        <v>45147</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="16">
+        <v>9094966111</v>
+      </c>
+      <c r="C15" s="16">
+        <v>2</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="19">
+        <v>45147</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="16">
+        <v>6601600025</v>
+      </c>
+      <c r="C16" s="16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="17">
+        <v>45159</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="16">
-        <v>6613500172</v>
-      </c>
-      <c r="C14" s="16">
-        <v>6</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="17">
-        <v>45143</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="I16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" s="22"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="16">
+        <v>6613600050</v>
+      </c>
+      <c r="C17" s="16">
+        <v>2</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="17">
+        <v>45159</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="16">
-        <v>93920565</v>
-      </c>
-      <c r="C15" s="16">
-        <v>40</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="17">
-        <v>45147</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="16">
-        <v>6613200160</v>
-      </c>
-      <c r="C16" s="16">
-        <v>40</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="19">
-        <v>45147</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="16">
-        <v>6613599160</v>
-      </c>
-      <c r="C17" s="16">
-        <v>3</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="19">
-        <v>45147</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I17" s="22" t="s">
-        <v>52</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="L17" s="22"/>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
       <c r="B18" s="16">
-        <v>9094966111</v>
+        <v>6613399229</v>
       </c>
       <c r="C18" s="16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="19">
+        <v>32</v>
+      </c>
+      <c r="E18" s="17">
         <v>45147</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="37"/>
+      <c r="G18" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+        <v>56</v>
+      </c>
+      <c r="L18" s="22"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
       <c r="B19" s="16">
-        <v>6601600025</v>
+        <v>6613399183</v>
       </c>
       <c r="C19" s="16">
+        <v>5</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="17">
+        <v>45147</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="25">
+        <v>9025119660</v>
+      </c>
+      <c r="C20" s="25">
+        <v>1</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="42">
+        <v>45255</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="25">
+        <v>1807002450</v>
+      </c>
+      <c r="C21" s="25">
         <v>2</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="17">
-        <v>45159</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="22"/>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="16">
-        <v>6613600050</v>
-      </c>
-      <c r="C20" s="16">
+      <c r="D21" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="43"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="25">
+        <v>1807002400</v>
+      </c>
+      <c r="C22" s="25">
         <v>2</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="17">
-        <v>45159</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="22"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="16">
-        <v>6613399229</v>
-      </c>
-      <c r="C21" s="16">
+      <c r="D22" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="42">
+        <v>45252</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="25">
+        <v>1807002500</v>
+      </c>
+      <c r="C23" s="25">
         <v>2</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="17">
-        <v>45147</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" s="22"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="16">
-        <v>6613399183</v>
-      </c>
-      <c r="C22" s="16">
-        <v>2</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="17">
-        <v>45147</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="L22" s="22"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="25">
-        <v>9025119660</v>
-      </c>
-      <c r="C23" s="25">
-        <v>1</v>
-      </c>
       <c r="D23" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="47">
-        <v>45255</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E23" s="44"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>59</v>
+      <c r="G23" s="32"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="25">
-        <v>1807002450</v>
+        <v>1807002700</v>
       </c>
       <c r="C24" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="48"/>
+        <v>66</v>
+      </c>
+      <c r="E24" s="43"/>
       <c r="F24" s="25"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="25">
-        <v>1807002400</v>
-      </c>
-      <c r="C25" s="25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="47">
-        <v>45252</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="25">
-        <v>1807002500</v>
-      </c>
-      <c r="C26" s="25">
-        <v>2</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="25">
-        <v>1807002700</v>
-      </c>
-      <c r="C27" s="25">
-        <v>4</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="48"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="1" t="s">
-        <v>74</v>
+      <c r="G24" s="32"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="A20:A24"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G19:G20"/>
     <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="A9:A19"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H5 H12:H23 H28:H1048576" xr:uid="{3C282085-0B6B-4E60-B943-5924EC8CC898}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H5 H9:H20 H25:H1048576" xr:uid="{3C282085-0B6B-4E60-B943-5924EC8CC898}">
       <formula1>"Doug,Dustin,Ethan,Patrick,Paul,Scott,Victor,Zac"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Must Select &quot;Yes&quot; or &quot;No&quot;" sqref="G1:G5 G12:G23 G28:G1048576" xr:uid="{634E274A-C89D-4417-893F-94DD38B0565E}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Must Select &quot;Yes&quot; or &quot;No&quot;" sqref="G1:G5 G9:G20 G25:G1048576" xr:uid="{634E274A-C89D-4417-893F-94DD38B0565E}">
       <formula1>"Driving,Picked,Issued"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>